<commit_message>
timing R vs py, docu update, feature_names, unit_tests
</commit_message>
<xml_diff>
--- a/orf/_R/py_vs_R_timing.xlsx
+++ b/orf/_R/py_vs_R_timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\switchdrive\Projects\ORF_Python\ORFpy\orf\_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EC1DB62-CA2C-46B7-A223-6BDCFE4F8E97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F745E9-0666-4032-9BCC-C30DE26438C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="270" windowWidth="25440" windowHeight="15390" xr2:uid="{975E3034-C860-463C-A5C5-570BC31C0E20}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[hh]:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="[hh]:mm:ss"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -147,7 +147,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -464,14 +464,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B053AB64-A6A3-4AFA-B534-C743DDEF559B}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -568,6 +569,14 @@
         <f>P4-O4</f>
         <v>9.374999935971573E-4</v>
       </c>
+      <c r="J4" s="2">
+        <f>S4-R4</f>
+        <v>4.6296292566694319E-5</v>
+      </c>
+      <c r="K4" s="2">
+        <f>U4-T4</f>
+        <v>1.0416666918899864E-4</v>
+      </c>
       <c r="M4" s="1">
         <v>44663.47760416667</v>
       </c>
@@ -579,6 +588,18 @@
       </c>
       <c r="P4" s="1">
         <v>44663.479351851849</v>
+      </c>
+      <c r="R4" s="1">
+        <v>44670.35633101852</v>
+      </c>
+      <c r="S4" s="1">
+        <v>44670.356377314813</v>
+      </c>
+      <c r="T4" s="1">
+        <v>44670.356412037036</v>
+      </c>
+      <c r="U4" s="1">
+        <v>44670.356516203705</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -604,15 +625,32 @@
         <v>19</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ref="H5:H11" si="0">N5-M5</f>
+        <f t="shared" ref="H5:I11" si="0">N5-M5</f>
         <v>4.9768518510973081E-4</v>
       </c>
       <c r="I5" s="2"/>
+      <c r="J5" s="2">
+        <f t="shared" ref="J5:J7" si="1">S5-R5</f>
+        <v>5.7870369346346706E-5</v>
+      </c>
+      <c r="K5" s="2"/>
       <c r="M5" s="1">
         <v>44663.479351851849</v>
       </c>
       <c r="N5" s="1">
         <v>44663.479849537034</v>
+      </c>
+      <c r="R5" s="1">
+        <v>44670.356516203705</v>
+      </c>
+      <c r="S5" s="1">
+        <v>44670.356574074074</v>
+      </c>
+      <c r="T5" s="1">
+        <v>44670.35659722222</v>
+      </c>
+      <c r="U5" s="1">
+        <v>44670.35670138889</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -645,6 +683,14 @@
         <f>P6-O6</f>
         <v>3.4722222335403785E-4</v>
       </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>5.7870370073942468E-4</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" ref="K5:K6" si="2">U6-T6</f>
+        <v>1.9907407404389232E-3</v>
+      </c>
       <c r="M6" s="1">
         <v>44663.480671296296</v>
       </c>
@@ -656,6 +702,18 @@
       </c>
       <c r="P6" s="1">
         <v>44663.481886574074</v>
+      </c>
+      <c r="R6" s="1">
+        <v>44670.35670138889</v>
+      </c>
+      <c r="S6" s="1">
+        <v>44670.35728009259</v>
+      </c>
+      <c r="T6" s="1">
+        <v>44670.357303240744</v>
+      </c>
+      <c r="U6" s="1">
+        <v>44670.359293981484</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -688,6 +746,11 @@
         <f>P7-O7</f>
         <v>0.20891203703649808</v>
       </c>
+      <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12966435185080627</v>
+      </c>
+      <c r="K7" s="2"/>
       <c r="M7" s="1">
         <v>44663.481886574074</v>
       </c>
@@ -699,6 +762,12 @@
       </c>
       <c r="P7" s="1">
         <v>44663.754224537035</v>
+      </c>
+      <c r="R7" s="1">
+        <v>44670.359293981484</v>
+      </c>
+      <c r="S7" s="1">
+        <v>44670.488958333335</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -731,6 +800,8 @@
         <f>P8-O8</f>
         <v>7.4999999997089617E-3</v>
       </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
       <c r="M8" s="1">
         <v>44663.754224537035</v>
       </c>
@@ -771,6 +842,8 @@
         <v>1.3657407398568466E-3</v>
       </c>
       <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
       <c r="M9" s="1">
         <v>44663.766215277778</v>
       </c>
@@ -808,6 +881,8 @@
         <f>P10-O10</f>
         <v>1.7939814788405783E-3</v>
       </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="M10" s="1">
         <v>44663.76939814815</v>
       </c>
@@ -847,7 +922,12 @@
         <f t="shared" si="0"/>
         <v>0.46194444444699911</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="2">
+        <f>P11-O11</f>
+        <v>3.3996412037013215</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="M11" s="1">
         <v>44663.773217592592</v>
       </c>
@@ -857,7 +937,9 @@
       <c r="O11" s="1">
         <v>44664.23574074074</v>
       </c>
-      <c r="P11" s="1"/>
+      <c r="P11" s="1">
+        <v>44667.635381944441</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>